<commit_message>
First working version of road trip map
</commit_message>
<xml_diff>
--- a/_drafts/road-trip/mileage.xlsx
+++ b/_drafts/road-trip/mileage.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claire/github/cduvallet.github.io/_drafts/road-trip/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claire/github/personal/cduvallet.github.io/_drafts/road-trip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B0015E-06EC-7748-A305-D6F1F206D185}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DD38E4-7FC8-AF4A-9B2A-51D2E563E6F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="1520" windowWidth="28040" windowHeight="16240" xr2:uid="{664FDB32-4895-0346-A745-EFF5A9847771}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16240" xr2:uid="{664FDB32-4895-0346-A745-EFF5A9847771}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -99,18 +99,12 @@
     <t>big bend hot springs</t>
   </si>
   <si>
-    <t>big bend</t>
-  </si>
-  <si>
     <t>morning</t>
   </si>
   <si>
     <t>austin</t>
   </si>
   <si>
-    <t>sam houton national forest</t>
-  </si>
-  <si>
     <t>talladega national forest</t>
   </si>
   <si>
@@ -349,6 +343,12 @@
   </si>
   <si>
     <t>whitehorse ranch ln</t>
+  </si>
+  <si>
+    <t>big bend national park</t>
+  </si>
+  <si>
+    <t>sam houston national forest</t>
   </si>
 </sst>
 </file>
@@ -703,11 +703,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1842507-326A-DE42-A4E6-0F43EB3A9456}">
   <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="32" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -726,7 +729,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H1" t="s">
         <v>17</v>
@@ -889,7 +892,7 @@
         <v>43519</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
@@ -898,13 +901,13 @@
         <v>42921</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -912,7 +915,7 @@
         <v>43519</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
@@ -929,7 +932,7 @@
         <v>43522</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
@@ -938,7 +941,7 @@
         <v>43484</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -949,7 +952,7 @@
         <v>43523</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="C12" t="s">
         <v>22</v>
@@ -958,7 +961,7 @@
         <v>43674</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -969,10 +972,10 @@
         <v>43527</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D13">
         <v>44487</v>
@@ -989,10 +992,10 @@
         <v>43528</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D14">
         <v>44577</v>
@@ -1009,10 +1012,10 @@
         <v>43528</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D15">
         <v>45361</v>
@@ -1029,10 +1032,10 @@
         <v>43529</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D16">
         <v>45706</v>
@@ -1049,10 +1052,10 @@
         <v>43563</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D17">
         <v>46562</v>
@@ -1069,16 +1072,16 @@
         <v>43564</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D18">
         <v>46891</v>
       </c>
       <c r="E18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F18">
         <v>2</v>
@@ -1089,10 +1092,10 @@
         <v>43564</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D19">
         <v>46996</v>
@@ -1109,16 +1112,16 @@
         <v>43565</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D20">
         <v>47237</v>
       </c>
       <c r="E20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F20">
         <v>2</v>
@@ -1129,10 +1132,10 @@
         <v>43565</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D21">
         <v>47515</v>
@@ -1149,10 +1152,10 @@
         <v>43565</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D22">
         <v>47552</v>
@@ -1169,10 +1172,10 @@
         <v>43565</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D23">
         <v>47733</v>
@@ -1189,10 +1192,10 @@
         <v>43571</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D24">
         <v>47743</v>
@@ -1209,10 +1212,10 @@
         <v>43571</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D25">
         <v>47959</v>
@@ -1229,10 +1232,10 @@
         <v>43571</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1246,10 +1249,10 @@
         <v>43572</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E27" t="s">
         <v>12</v>
@@ -1263,10 +1266,10 @@
         <v>43572</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D28">
         <v>48259</v>
@@ -1283,10 +1286,10 @@
         <v>43573</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E29" t="s">
         <v>7</v>
@@ -1300,16 +1303,16 @@
         <v>43574</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D30">
         <v>48406</v>
       </c>
       <c r="E30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F30">
         <v>2</v>
@@ -1320,16 +1323,16 @@
         <v>43575</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C31" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D31">
         <v>48818</v>
       </c>
       <c r="E31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F31">
         <v>2</v>
@@ -1340,7 +1343,7 @@
         <v>43575</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C32" t="s">
         <v>22</v>
@@ -1360,16 +1363,16 @@
         <v>43576</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D33">
         <v>49068</v>
       </c>
       <c r="E33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F33">
         <v>2</v>
@@ -1380,10 +1383,10 @@
         <v>43576</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D34">
         <v>49295</v>
@@ -1400,10 +1403,10 @@
         <v>43577</v>
       </c>
       <c r="B35" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C35" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D35">
         <v>49600</v>
@@ -1420,10 +1423,10 @@
         <v>43578</v>
       </c>
       <c r="B36" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C36" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D36">
         <v>49650</v>
@@ -1440,10 +1443,10 @@
         <v>43578</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D37">
         <v>49788</v>
@@ -1460,7 +1463,7 @@
         <v>43579</v>
       </c>
       <c r="B38" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C38" t="s">
         <v>9</v>
@@ -1477,7 +1480,7 @@
         <v>43580</v>
       </c>
       <c r="B39" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C39" t="s">
         <v>9</v>
@@ -1497,7 +1500,7 @@
         <v>43581</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C40" t="s">
         <v>9</v>
@@ -1517,13 +1520,13 @@
         <v>43582</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C41" t="s">
         <v>9</v>
       </c>
       <c r="E41" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F41">
         <v>2</v>
@@ -1534,7 +1537,7 @@
         <v>43583</v>
       </c>
       <c r="B42" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C42" t="s">
         <v>9</v>
@@ -1554,7 +1557,7 @@
         <v>43584</v>
       </c>
       <c r="B43" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C43" t="s">
         <v>9</v>
@@ -1574,7 +1577,7 @@
         <v>43585</v>
       </c>
       <c r="B44" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C44" t="s">
         <v>9</v>
@@ -1583,7 +1586,7 @@
         <v>50450</v>
       </c>
       <c r="E44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F44">
         <v>2</v>
@@ -1594,10 +1597,10 @@
         <v>43586</v>
       </c>
       <c r="B45" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C45" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D45">
         <v>50562</v>
@@ -1614,16 +1617,16 @@
         <v>43587</v>
       </c>
       <c r="B46" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C46" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D46">
         <v>50659</v>
       </c>
       <c r="E46" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F46">
         <v>2</v>
@@ -1634,10 +1637,10 @@
         <v>43587</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C47" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D47">
         <v>50691</v>
@@ -1654,10 +1657,10 @@
         <v>43587</v>
       </c>
       <c r="B48" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C48" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D48">
         <v>50769</v>
@@ -1674,10 +1677,10 @@
         <v>43588</v>
       </c>
       <c r="B49" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C49" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E49" t="s">
         <v>7</v>
@@ -1691,10 +1694,10 @@
         <v>43588</v>
       </c>
       <c r="B50" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C50" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E50" t="s">
         <v>10</v>
@@ -1708,13 +1711,13 @@
         <v>43589</v>
       </c>
       <c r="B51" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C51" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F51">
         <v>2</v>
@@ -1725,16 +1728,16 @@
         <v>43590</v>
       </c>
       <c r="B52" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C52" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D52">
         <v>50932</v>
       </c>
       <c r="E52" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F52">
         <v>2</v>
@@ -1745,10 +1748,10 @@
         <v>43590</v>
       </c>
       <c r="B53" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C53" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D53">
         <v>50980</v>
@@ -1765,10 +1768,10 @@
         <v>43591</v>
       </c>
       <c r="B54" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C54" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D54">
         <v>51068</v>
@@ -1785,10 +1788,10 @@
         <v>43591</v>
       </c>
       <c r="B55" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C55" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D55">
         <v>51144</v>
@@ -1805,10 +1808,10 @@
         <v>43592</v>
       </c>
       <c r="B56" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C56" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D56">
         <v>51298</v>
@@ -1825,16 +1828,16 @@
         <v>43593</v>
       </c>
       <c r="B57" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C57" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D57">
         <v>51372</v>
       </c>
       <c r="E57" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F57">
         <v>2</v>
@@ -1845,10 +1848,10 @@
         <v>43593</v>
       </c>
       <c r="B58" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C58" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D58">
         <v>51434</v>
@@ -1865,16 +1868,16 @@
         <v>43594</v>
       </c>
       <c r="B59" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C59" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D59">
         <v>51507</v>
       </c>
       <c r="E59" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F59">
         <v>2</v>
@@ -1885,10 +1888,10 @@
         <v>43594</v>
       </c>
       <c r="B60" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C60" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D60">
         <v>51930</v>
@@ -1905,16 +1908,16 @@
         <v>43595</v>
       </c>
       <c r="B61" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C61" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D61">
         <v>51945</v>
       </c>
       <c r="E61" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F61">
         <v>2</v>
@@ -1925,10 +1928,10 @@
         <v>43595</v>
       </c>
       <c r="B62" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C62" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E62" t="s">
         <v>10</v>
@@ -1942,13 +1945,13 @@
         <v>43596</v>
       </c>
       <c r="B63" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C63" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E63" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F63">
         <v>2</v>
@@ -1959,13 +1962,13 @@
         <v>43597</v>
       </c>
       <c r="B64" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C64" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E64" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F64">
         <v>2</v>
@@ -1976,13 +1979,13 @@
         <v>43598</v>
       </c>
       <c r="B65" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C65" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E65" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F65">
         <v>2</v>
@@ -1993,10 +1996,10 @@
         <v>43599</v>
       </c>
       <c r="B66" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C66" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E66" t="s">
         <v>14</v>
@@ -2010,16 +2013,16 @@
         <v>43600</v>
       </c>
       <c r="B67" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C67" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D67">
         <v>52238</v>
       </c>
       <c r="E67" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F67">
         <v>2</v>
@@ -2030,10 +2033,10 @@
         <v>43600</v>
       </c>
       <c r="B68" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C68" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D68">
         <v>52251</v>
@@ -2050,10 +2053,10 @@
         <v>43600</v>
       </c>
       <c r="B69" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C69" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D69">
         <v>52340</v>
@@ -2070,10 +2073,10 @@
         <v>43601</v>
       </c>
       <c r="B70" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C70" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D70">
         <v>52381</v>
@@ -2090,10 +2093,10 @@
         <v>43601</v>
       </c>
       <c r="B71" t="s">
+        <v>80</v>
+      </c>
+      <c r="C71" t="s">
         <v>82</v>
-      </c>
-      <c r="C71" t="s">
-        <v>84</v>
       </c>
       <c r="D71">
         <v>52606</v>
@@ -2110,10 +2113,10 @@
         <v>43602</v>
       </c>
       <c r="B72" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C72" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E72" t="s">
         <v>7</v>
@@ -2127,13 +2130,13 @@
         <v>43603</v>
       </c>
       <c r="B73" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C73" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E73" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F73">
         <v>2</v>
@@ -2144,16 +2147,16 @@
         <v>43604</v>
       </c>
       <c r="B74" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C74" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D74">
         <v>52822</v>
       </c>
       <c r="E74" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F74">
         <v>2</v>
@@ -2164,16 +2167,16 @@
         <v>43605</v>
       </c>
       <c r="B75" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C75" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D75">
         <v>53034</v>
       </c>
       <c r="E75" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F75">
         <v>2</v>
@@ -2184,10 +2187,10 @@
         <v>43605</v>
       </c>
       <c r="B76" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C76" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D76">
         <v>53067</v>
@@ -2204,10 +2207,10 @@
         <v>43605</v>
       </c>
       <c r="B77" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C77" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D77">
         <v>53321</v>
@@ -2224,16 +2227,16 @@
         <v>43606</v>
       </c>
       <c r="B78" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C78" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D78">
         <v>53407</v>
       </c>
       <c r="E78" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F78">
         <v>2</v>
@@ -2244,10 +2247,10 @@
         <v>43606</v>
       </c>
       <c r="B79" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C79" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D79">
         <v>53515</v>
@@ -2264,10 +2267,10 @@
         <v>43606</v>
       </c>
       <c r="B80" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C80" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D80">
         <v>53540</v>
@@ -2284,10 +2287,10 @@
         <v>43607</v>
       </c>
       <c r="B81" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C81" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D81">
         <v>53594</v>
@@ -2304,10 +2307,10 @@
         <v>43607</v>
       </c>
       <c r="B82" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C82" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D82">
         <v>53677</v>
@@ -2324,10 +2327,10 @@
         <v>43608</v>
       </c>
       <c r="B83" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C83" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D83">
         <v>53730</v>
@@ -2344,10 +2347,10 @@
         <v>43608</v>
       </c>
       <c r="B84" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C84" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D84">
         <v>53822</v>
@@ -2364,10 +2367,10 @@
         <v>43608</v>
       </c>
       <c r="B85" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C85" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D85">
         <v>54100</v>
@@ -2384,10 +2387,10 @@
         <v>43609</v>
       </c>
       <c r="B86" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C86" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D86">
         <v>54148</v>
@@ -2404,10 +2407,10 @@
         <v>43609</v>
       </c>
       <c r="B87" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C87" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E87" t="s">
         <v>7</v>
@@ -2421,10 +2424,10 @@
         <v>43609</v>
       </c>
       <c r="B88" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C88" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D88">
         <v>54386</v>
@@ -2441,13 +2444,13 @@
         <v>43610</v>
       </c>
       <c r="B89" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C89" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E89" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F89">
         <v>2</v>
@@ -2458,13 +2461,13 @@
         <v>43611</v>
       </c>
       <c r="B90" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C90" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E90" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F90">
         <v>2</v>
@@ -2475,16 +2478,16 @@
         <v>43612</v>
       </c>
       <c r="B91" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C91" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D91">
         <v>54386</v>
       </c>
       <c r="E91" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F91">
         <v>2</v>
@@ -2495,7 +2498,7 @@
         <v>43612</v>
       </c>
       <c r="B92" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C92" t="s">
         <v>6</v>
@@ -2515,13 +2518,13 @@
         <v>43613</v>
       </c>
       <c r="B93" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C93" t="s">
         <v>6</v>
       </c>
       <c r="E93" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F93">
         <v>2</v>
@@ -2532,7 +2535,7 @@
         <v>43614</v>
       </c>
       <c r="B94" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C94" t="s">
         <v>6</v>
@@ -2541,7 +2544,7 @@
         <v>54573</v>
       </c>
       <c r="E94" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F94">
         <v>2</v>
@@ -2552,7 +2555,7 @@
         <v>43615</v>
       </c>
       <c r="B95" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C95" t="s">
         <v>6</v>
@@ -2569,7 +2572,7 @@
         <v>43616</v>
       </c>
       <c r="B96" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C96" t="s">
         <v>6</v>
@@ -2589,7 +2592,7 @@
         <v>43617</v>
       </c>
       <c r="B97" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C97" t="s">
         <v>6</v>
@@ -2609,7 +2612,7 @@
         <v>43617</v>
       </c>
       <c r="B98" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C98" t="s">
         <v>6</v>

</xml_diff>